<commit_message>
Added standard deviation to excel report.
</commit_message>
<xml_diff>
--- a/src/ExcelRendering/PerformanceTemplate.xlsx
+++ b/src/ExcelRendering/PerformanceTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Performance</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>1 Yr Std Dev</t>
   </si>
 </sst>
 </file>
@@ -402,9 +405,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -415,14 +420,15 @@
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -446,6 +452,9 @@
       </c>
       <c r="H4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 6 months and started on quarter to date
</commit_message>
<xml_diff>
--- a/src/ExcelRendering/PerformanceTemplate.xlsx
+++ b/src/ExcelRendering/PerformanceTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="27792" windowHeight="12072"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Performance</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Year to Date</t>
-  </si>
-  <si>
     <t>12 Month</t>
   </si>
   <si>
@@ -41,6 +38,15 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>6 Month</t>
+  </si>
+  <si>
+    <t>Year To Date</t>
+  </si>
+  <si>
+    <t>Quarter To Date</t>
   </si>
 </sst>
 </file>
@@ -402,50 +408,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented excel for standard deviation
</commit_message>
<xml_diff>
--- a/src/ExcelRendering/PerformanceTemplate.xlsx
+++ b/src/ExcelRendering/PerformanceTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Performance</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Quarter To Date</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,15 +427,16 @@
     <col min="7" max="7" width="15.44140625" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="11" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -462,6 +466,9 @@
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added eman to excel, added mean to portfolio, removed std from benchmarks
</commit_message>
<xml_diff>
--- a/src/ExcelRendering/PerformanceTemplate.xlsx
+++ b/src/ExcelRendering/PerformanceTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Performance</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,12 +434,12 @@
     <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -469,6 +472,9 @@
       </c>
       <c r="K4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>